<commit_message>
Parts Expert Skill Value Bug Fix
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186A07DA-91D1-47B2-94BA-E1A4C62A7EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A2D264-75A8-4947-B81B-61CDD80FD3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="555" windowWidth="19425" windowHeight="11835" activeTab="1" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" activeTab="5" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -916,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A79C965-7C44-4D18-8FA2-EDE3E862FC28}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -3872,7 +3861,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3927,7 +3916,7 @@
         <v>0.4</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f>D2+200</f>
@@ -4381,7 +4370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ADB55A-26D1-4F0B-80EF-12E94A5233E5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -4883,7 +4872,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4938,7 +4927,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f>D2+200</f>
@@ -5383,8 +5372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80A1835-1FAB-40B8-8AD8-8B530C837E11}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5439,7 +5428,7 @@
         <v>0.02</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f>D2+200</f>

</xml_diff>

<commit_message>
Revert "Parts Expert Skill Value Bug Fix"
This reverts commit 2a400b100be3bda8c43bc08898394cb9087e82bb.
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\cosmos\Assets\8. Execl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A2D264-75A8-4947-B81B-61CDD80FD3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186A07DA-91D1-47B2-94BA-E1A4C62A7EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" activeTab="5" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
+    <workbookView xWindow="-90" yWindow="555" windowWidth="19425" windowHeight="11835" activeTab="1" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -905,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A79C965-7C44-4D18-8FA2-EDE3E862FC28}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -3861,7 +3872,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3916,7 +3927,7 @@
         <v>0.4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f>D2+200</f>
@@ -4370,7 +4381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ADB55A-26D1-4F0B-80EF-12E94A5233E5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -4872,7 +4883,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4927,7 +4938,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f>D2+200</f>
@@ -5372,8 +5383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80A1835-1FAB-40B8-8AD8-8B530C837E11}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5428,7 +5439,7 @@
         <v>0.02</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f>D2+200</f>

</xml_diff>

<commit_message>
Wave Balancing 04.25 (2)
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubDesktop\cosmos\Assets\8. Execl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE762418-E8EE-43F2-9955-042C5D066FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="555" windowWidth="19425" windowHeight="11835" activeTab="5"/>
+    <workbookView xWindow="2040" yWindow="1605" windowWidth="19425" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Laser" sheetId="5" r:id="rId5"/>
     <sheet name="Emp" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -297,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -678,7 +679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -923,11 +924,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1069,7 +1070,7 @@
       </c>
       <c r="B3">
         <f>B2+0.2</f>
-        <v>1.2</v>
+        <v>2.6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1136,7 +1137,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B10" si="1">B3+0.2</f>
-        <v>1.4</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1203,7 +1204,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>1.5999999999999999</v>
+        <v>3.0000000000000004</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1270,7 +1271,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
+        <v>3.2000000000000006</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1339,7 +1340,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>1.9999999999999998</v>
+        <v>3.4000000000000008</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1408,7 +1409,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>2.1999999999999997</v>
+        <v>3.600000000000001</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1477,7 +1478,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>2.4</v>
+        <v>3.8000000000000012</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1546,7 +1547,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>2.6</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1680,7 +1681,7 @@
       </c>
       <c r="B12">
         <f>B10+0.2</f>
-        <v>2.8000000000000003</v>
+        <v>4.2000000000000011</v>
       </c>
       <c r="C12">
         <f>C2*2</f>
@@ -1753,7 +1754,7 @@
       </c>
       <c r="B13">
         <f>B12+0.2</f>
-        <v>3.0000000000000004</v>
+        <v>4.4000000000000012</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:D20" si="4">C3*2</f>
@@ -1825,7 +1826,7 @@
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B20" si="6">B13+0.2</f>
-        <v>3.2000000000000006</v>
+        <v>4.6000000000000014</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
@@ -1897,7 +1898,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="6"/>
-        <v>3.4000000000000008</v>
+        <v>4.8000000000000016</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
@@ -1971,7 +1972,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="6"/>
-        <v>3.600000000000001</v>
+        <v>5.0000000000000018</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
@@ -2045,7 +2046,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="6"/>
-        <v>3.8000000000000012</v>
+        <v>5.200000000000002</v>
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
@@ -2119,7 +2120,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="6"/>
-        <v>4.0000000000000009</v>
+        <v>5.4000000000000021</v>
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
@@ -2193,7 +2194,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="6"/>
-        <v>4.2000000000000011</v>
+        <v>5.6000000000000023</v>
       </c>
       <c r="C19">
         <f t="shared" si="4"/>
@@ -2267,7 +2268,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="6"/>
-        <v>4.4000000000000012</v>
+        <v>5.8000000000000025</v>
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
@@ -2406,7 +2407,7 @@
       </c>
       <c r="B22">
         <f>B20+0.2</f>
-        <v>4.6000000000000014</v>
+        <v>6.0000000000000027</v>
       </c>
       <c r="C22">
         <f>C12*2</f>
@@ -2478,7 +2479,7 @@
       </c>
       <c r="B23">
         <f>B22+0.2</f>
-        <v>4.8000000000000016</v>
+        <v>6.2000000000000028</v>
       </c>
       <c r="C23">
         <f t="shared" ref="C23:D30" si="12">C13*2</f>
@@ -2551,7 +2552,7 @@
       </c>
       <c r="B24">
         <f t="shared" ref="B24:B30" si="14">B23+0.2</f>
-        <v>5.0000000000000018</v>
+        <v>6.400000000000003</v>
       </c>
       <c r="C24">
         <f t="shared" si="12"/>
@@ -2624,7 +2625,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="14"/>
-        <v>5.200000000000002</v>
+        <v>6.6000000000000032</v>
       </c>
       <c r="C25">
         <f t="shared" si="12"/>
@@ -2699,7 +2700,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="14"/>
-        <v>5.4000000000000021</v>
+        <v>6.8000000000000034</v>
       </c>
       <c r="C26">
         <f t="shared" si="12"/>
@@ -2774,7 +2775,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="14"/>
-        <v>5.6000000000000023</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="C27">
         <f t="shared" si="12"/>
@@ -2849,7 +2850,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="14"/>
-        <v>5.8000000000000025</v>
+        <v>7.2000000000000037</v>
       </c>
       <c r="C28">
         <f t="shared" si="12"/>
@@ -2924,7 +2925,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="14"/>
-        <v>6.0000000000000027</v>
+        <v>7.4000000000000039</v>
       </c>
       <c r="C29">
         <f t="shared" si="12"/>
@@ -2999,7 +3000,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="14"/>
-        <v>6.2000000000000028</v>
+        <v>7.6000000000000041</v>
       </c>
       <c r="C30">
         <f t="shared" si="12"/>
@@ -3139,7 +3140,7 @@
       </c>
       <c r="B32">
         <f>B30+0.2</f>
-        <v>6.400000000000003</v>
+        <v>7.8000000000000043</v>
       </c>
       <c r="C32">
         <f>C22*2</f>
@@ -3213,7 +3214,7 @@
       </c>
       <c r="B33">
         <f>B32+0.2</f>
-        <v>6.6000000000000032</v>
+        <v>8.0000000000000036</v>
       </c>
       <c r="C33">
         <f t="shared" ref="C33:D40" si="21">C23*2</f>
@@ -3288,7 +3289,7 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:B40" si="23">B33+0.2</f>
-        <v>6.8000000000000034</v>
+        <v>8.2000000000000028</v>
       </c>
       <c r="C34">
         <f t="shared" si="21"/>
@@ -3363,7 +3364,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="23"/>
-        <v>7.0000000000000036</v>
+        <v>8.4000000000000021</v>
       </c>
       <c r="C35">
         <f t="shared" si="21"/>
@@ -3438,7 +3439,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="23"/>
-        <v>7.2000000000000037</v>
+        <v>8.6000000000000014</v>
       </c>
       <c r="C36">
         <f t="shared" si="21"/>
@@ -3513,7 +3514,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="23"/>
-        <v>7.4000000000000039</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C37">
         <f t="shared" si="21"/>
@@ -3588,7 +3589,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="23"/>
-        <v>7.6000000000000041</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <f t="shared" si="21"/>
@@ -3663,7 +3664,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="23"/>
-        <v>7.8000000000000043</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C39">
         <f t="shared" si="21"/>
@@ -3738,7 +3739,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="23"/>
-        <v>8.0000000000000036</v>
+        <v>9.3999999999999986</v>
       </c>
       <c r="C40">
         <f t="shared" si="21"/>
@@ -3878,10 +3879,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4388,7 +4389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4443,7 +4444,7 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="B3">
-        <f>B2-0.025</f>
+        <f t="shared" ref="B3:B21" si="0">B2-0.025</f>
         <v>0.75</v>
       </c>
       <c r="C3">
@@ -4463,22 +4464,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="0">A3+0.025</f>
+        <f t="shared" ref="A4:A21" si="1">A3+0.025</f>
         <v>0.1</v>
       </c>
       <c r="B4">
-        <f>B3-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="C4">
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="1">D3+200</f>
+        <f t="shared" ref="D4:D20" si="2">D3+200</f>
         <v>900</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="2">E3+200</f>
+        <f t="shared" ref="E4:E20" si="3">E3+200</f>
         <v>900</v>
       </c>
       <c r="F4">
@@ -4487,22 +4488,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
       <c r="B5">
-        <f>B4-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
       <c r="F5">
@@ -4511,22 +4512,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
       <c r="B6">
-        <f>B5-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.67499999999999993</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
       <c r="F6">
@@ -4535,22 +4536,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="B7">
-        <f>B6-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.64999999999999991</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1500</v>
       </c>
       <c r="F7">
@@ -4559,22 +4560,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="B8">
-        <f>B7-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.62499999999999989</v>
       </c>
       <c r="C8">
         <v>-1</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1700</v>
       </c>
       <c r="F8">
@@ -4583,22 +4584,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22499999999999998</v>
       </c>
       <c r="B9">
-        <f>B8-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.59999999999999987</v>
       </c>
       <c r="C9">
         <v>-1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1900</v>
       </c>
       <c r="F9">
@@ -4607,22 +4608,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="B10">
-        <f>B9-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.57499999999999984</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2100</v>
       </c>
       <c r="F10">
@@ -4631,22 +4632,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.27499999999999997</v>
       </c>
       <c r="B11">
-        <f>B10-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.54999999999999982</v>
       </c>
       <c r="C11">
         <v>-1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2300</v>
       </c>
       <c r="F11">
@@ -4655,22 +4656,22 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="B12">
-        <f>B11-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.5249999999999998</v>
       </c>
       <c r="C12">
         <v>-1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2500</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
       <c r="F12">
@@ -4679,22 +4680,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="B13">
-        <f>B12-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.49999999999999978</v>
       </c>
       <c r="C13">
         <v>-1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2700</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2700</v>
       </c>
       <c r="F13">
@@ -4703,22 +4704,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="B14">
-        <f>B13-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.47499999999999976</v>
       </c>
       <c r="C14">
         <v>-1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2900</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2900</v>
       </c>
       <c r="F14">
@@ -4727,22 +4728,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37500000000000006</v>
       </c>
       <c r="B15">
-        <f>B14-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.44999999999999973</v>
       </c>
       <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3100</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3100</v>
       </c>
       <c r="F15">
@@ -4751,22 +4752,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40000000000000008</v>
       </c>
       <c r="B16">
-        <f>B15-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.42499999999999971</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3300</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3300</v>
       </c>
       <c r="F16">
@@ -4775,22 +4776,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4250000000000001</v>
       </c>
       <c r="B17">
-        <f>B16-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.39999999999999969</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3500</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3500</v>
       </c>
       <c r="F17">
@@ -4799,22 +4800,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.45000000000000012</v>
       </c>
       <c r="B18">
-        <f>B17-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.37499999999999967</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3700</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3700</v>
       </c>
       <c r="F18">
@@ -4823,22 +4824,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47500000000000014</v>
       </c>
       <c r="B19">
-        <f>B18-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.34999999999999964</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3900</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3900</v>
       </c>
       <c r="F19">
@@ -4847,22 +4848,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.50000000000000011</v>
       </c>
       <c r="B20">
-        <f>B19-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.32499999999999962</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4100</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4100</v>
       </c>
       <c r="F20">
@@ -4871,11 +4872,11 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.52500000000000013</v>
       </c>
       <c r="B21">
-        <f>B20-0.025</f>
+        <f t="shared" si="0"/>
         <v>0.2999999999999996</v>
       </c>
       <c r="C21">
@@ -4889,7 +4890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4968,18 +4969,18 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <f>B3+0.1</f>
+        <f t="shared" ref="B4:B21" si="1">B3+0.1</f>
         <v>0.5</v>
       </c>
       <c r="C4">
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="1">D3+200</f>
+        <f t="shared" ref="D4:D20" si="2">D3+200</f>
         <v>900</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="2">E3+200</f>
+        <f t="shared" ref="E4:E20" si="3">E3+200</f>
         <v>900</v>
       </c>
       <c r="F4">
@@ -4992,18 +4993,18 @@
         <v>0.6</v>
       </c>
       <c r="B5">
-        <f>B4+0.1</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
       <c r="F5">
@@ -5016,18 +5017,18 @@
         <v>0.7</v>
       </c>
       <c r="B6">
-        <f>B5+0.1</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
       <c r="F6">
@@ -5040,18 +5041,18 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="B7">
-        <f>B6+0.1</f>
+        <f t="shared" si="1"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1500</v>
       </c>
       <c r="F7">
@@ -5064,18 +5065,18 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="B8">
-        <f>B7+0.1</f>
+        <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="C8">
         <v>-1</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1700</v>
       </c>
       <c r="F8">
@@ -5088,18 +5089,18 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="B9">
-        <f>B8+0.1</f>
+        <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="C9">
         <v>-1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1900</v>
       </c>
       <c r="F9">
@@ -5112,18 +5113,18 @@
         <v>1.0999999999999999</v>
       </c>
       <c r="B10">
-        <f>B9+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2100</v>
       </c>
       <c r="F10">
@@ -5136,18 +5137,18 @@
         <v>1.2</v>
       </c>
       <c r="B11">
-        <f>B10+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="C11">
         <v>-1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2300</v>
       </c>
       <c r="F11">
@@ -5160,18 +5161,18 @@
         <v>1.3</v>
       </c>
       <c r="B12">
-        <f>B11+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="C12">
         <v>-1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2500</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
       <c r="F12">
@@ -5184,18 +5185,18 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="B13">
-        <f>B12+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="C13">
         <v>-1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2700</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2700</v>
       </c>
       <c r="F13">
@@ -5208,18 +5209,18 @@
         <v>1.5000000000000002</v>
       </c>
       <c r="B14">
-        <f>B13+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="C14">
         <v>-1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2900</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2900</v>
       </c>
       <c r="F14">
@@ -5232,18 +5233,18 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="B15">
-        <f>B14+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.6000000000000003</v>
       </c>
       <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3100</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3100</v>
       </c>
       <c r="F15">
@@ -5256,18 +5257,18 @@
         <v>1.7000000000000004</v>
       </c>
       <c r="B16">
-        <f>B15+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.7000000000000004</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3300</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3300</v>
       </c>
       <c r="F16">
@@ -5280,18 +5281,18 @@
         <v>1.8000000000000005</v>
       </c>
       <c r="B17">
-        <f>B16+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.8000000000000005</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3500</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3500</v>
       </c>
       <c r="F17">
@@ -5304,18 +5305,18 @@
         <v>1.9000000000000006</v>
       </c>
       <c r="B18">
-        <f>B17+0.1</f>
+        <f t="shared" si="1"/>
         <v>1.9000000000000006</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3700</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3700</v>
       </c>
       <c r="F18">
@@ -5328,18 +5329,18 @@
         <v>2.0000000000000004</v>
       </c>
       <c r="B19">
-        <f>B18+0.1</f>
+        <f t="shared" si="1"/>
         <v>2.0000000000000004</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3900</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3900</v>
       </c>
       <c r="F19">
@@ -5352,18 +5353,18 @@
         <v>2.1000000000000005</v>
       </c>
       <c r="B20">
-        <f>B19+0.1</f>
+        <f t="shared" si="1"/>
         <v>2.1000000000000005</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4100</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4100</v>
       </c>
       <c r="F20">
@@ -5376,7 +5377,7 @@
         <v>2.2000000000000006</v>
       </c>
       <c r="B21">
-        <f>B20+0.1</f>
+        <f t="shared" si="1"/>
         <v>2.2000000000000006</v>
       </c>
       <c r="C21">
@@ -5390,10 +5391,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -5445,7 +5446,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="B3">
-        <f>B2+0.005</f>
+        <f t="shared" ref="B3:B21" si="0">B2+0.005</f>
         <v>0.255</v>
       </c>
       <c r="C3">
@@ -5465,22 +5466,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="0">A3+0.025</f>
+        <f t="shared" ref="A4:A21" si="1">A3+0.025</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="B4">
-        <f>B3+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
       <c r="C4">
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="1">D3+200</f>
+        <f t="shared" ref="D4:D20" si="2">D3+200</f>
         <v>900</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="2">E3+200</f>
+        <f t="shared" ref="E4:E20" si="3">E3+200</f>
         <v>900</v>
       </c>
       <c r="F4">
@@ -5489,22 +5490,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22499999999999998</v>
       </c>
       <c r="B5">
-        <f>B4+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.26500000000000001</v>
       </c>
       <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
       <c r="F5">
@@ -5513,22 +5514,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="B6">
-        <f>B5+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
       <c r="F6">
@@ -5537,22 +5538,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.27499999999999997</v>
       </c>
       <c r="B7">
-        <f>B6+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1500</v>
       </c>
       <c r="F7">
@@ -5561,22 +5562,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="B8">
-        <f>B7+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="C8">
         <v>-1</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1700</v>
       </c>
       <c r="F8">
@@ -5585,22 +5586,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="B9">
-        <f>B8+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.28500000000000003</v>
       </c>
       <c r="C9">
         <v>-1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1900</v>
       </c>
       <c r="F9">
@@ -5609,22 +5610,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="B10">
-        <f>B9+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2100</v>
       </c>
       <c r="F10">
@@ -5633,22 +5634,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37500000000000006</v>
       </c>
       <c r="B11">
-        <f>B10+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.29500000000000004</v>
       </c>
       <c r="C11">
         <v>-1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2300</v>
       </c>
       <c r="F11">
@@ -5657,22 +5658,22 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40000000000000008</v>
       </c>
       <c r="B12">
-        <f>B11+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="C12">
         <v>-1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2500</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
       <c r="F12">
@@ -5681,22 +5682,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4250000000000001</v>
       </c>
       <c r="B13">
-        <f>B12+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.30500000000000005</v>
       </c>
       <c r="C13">
         <v>-1</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2700</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2700</v>
       </c>
       <c r="F13">
@@ -5705,22 +5706,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.45000000000000012</v>
       </c>
       <c r="B14">
-        <f>B13+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="C14">
         <v>-1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2900</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2900</v>
       </c>
       <c r="F14">
@@ -5729,22 +5730,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47500000000000014</v>
       </c>
       <c r="B15">
-        <f>B14+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.31500000000000006</v>
       </c>
       <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3100</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3100</v>
       </c>
       <c r="F15">
@@ -5753,22 +5754,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.50000000000000011</v>
       </c>
       <c r="B16">
-        <f>B15+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3300</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3300</v>
       </c>
       <c r="F16">
@@ -5777,22 +5778,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.52500000000000013</v>
       </c>
       <c r="B17">
-        <f>B16+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.32500000000000007</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3500</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3500</v>
       </c>
       <c r="F17">
@@ -5801,22 +5802,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.55000000000000016</v>
       </c>
       <c r="B18">
-        <f>B17+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.33000000000000007</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3700</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3700</v>
       </c>
       <c r="F18">
@@ -5825,22 +5826,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57500000000000018</v>
       </c>
       <c r="B19">
-        <f>B18+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.33500000000000008</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3900</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3900</v>
       </c>
       <c r="F19">
@@ -5849,22 +5850,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6000000000000002</v>
       </c>
       <c r="B20">
-        <f>B19+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.34000000000000008</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4100</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4100</v>
       </c>
       <c r="F20">
@@ -5873,11 +5874,11 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.62500000000000022</v>
       </c>
       <c r="B21">
-        <f>B20+0.005</f>
+        <f t="shared" si="0"/>
         <v>0.34500000000000008</v>
       </c>
       <c r="C21">

</xml_diff>

<commit_message>
Excel Database 4 phase
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE762418-E8EE-43F2-9955-042C5D066FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319A0511-B1D1-4434-983A-A86AC6CF1A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1605" windowWidth="19425" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1605" windowWidth="19425" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -255,43 +255,42 @@
     <t>expertSkillUpgradeJem</t>
   </si>
   <si>
-    <t>1000,2000,3000,4000,5000</t>
+    <t>3000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>500,1000,1500,2000,2500</t>
+    <t>1000,2000,3000,4000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>500,1000,1500,2000,2500</t>
+    <t>500,1000,1500,2000</t>
+  </si>
+  <si>
+    <t>500,1000,1500,2000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>100,200,300,400,500</t>
+    <t>100,200,300,400</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>100,300,500,700,900</t>
+    <t>100,300,500,700</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>5,10,15,20,25</t>
+    <t>5,10,15,20</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>4,8,12,16,20</t>
+    <t>4,8,12,16</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>3,6,9,12,15</t>
+    <t>3,6,9,12</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2,5,8,11,14</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000</t>
+    <t>2,5,8,11</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -682,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -720,13 +719,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -736,11 +735,11 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
-        <v>5</v>
+      <c r="C3" s="3">
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>59</v>
@@ -753,11 +752,11 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>5</v>
+      <c r="C4" s="3">
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>59</v>
@@ -770,11 +769,11 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
-        <v>5</v>
+      <c r="C5" s="3">
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>59</v>
@@ -787,11 +786,11 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
-        <v>5</v>
+      <c r="C6" s="3">
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>59</v>
@@ -804,11 +803,11 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
-        <v>5</v>
+      <c r="C7" s="3">
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>59</v>
@@ -821,11 +820,11 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>5</v>
+      <c r="C8" s="3">
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>59</v>
@@ -838,11 +837,11 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
-        <v>5</v>
+      <c r="C9" s="3">
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>59</v>
@@ -862,7 +861,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,7 +878,7 @@
         <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -896,7 +895,7 @@
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -913,7 +912,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Hidden Mission Description Update
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0BFD20-1FA7-45AC-93AA-BFF4D387130B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5657260C-02CA-4996-9C7B-DA25E6B53EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1605" windowWidth="19425" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>achieveName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -137,13 +126,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>?????????????</t>
-  </si>
-  <si>
-    <t>?????????????</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>StarWars</t>
   </si>
   <si>
@@ -291,6 +273,22 @@
   </si>
   <si>
     <t>2,5,8,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All in game status level 30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 Parts all Unlocked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP Lv 50, Recovery Lv 50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Survive 30 Sec in Bouns Wave</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -681,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -722,10 +720,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -739,10 +737,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -756,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -773,10 +771,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -790,10 +788,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -807,10 +805,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -824,10 +822,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -841,10 +839,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -852,16 +850,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -869,16 +867,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -886,33 +884,33 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -937,67 +935,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>43</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>47</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>48</v>
-      </c>
-      <c r="T1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -3892,22 +3890,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4402,22 +4400,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4903,22 +4901,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -5404,22 +5402,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Missile Balancing Finish, (Boss, Wave ~ing)
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubDesktop\cosmos\Assets\8. Execl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA6B746-F1B5-4BCD-A1EF-1F37C4A6E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1605" windowWidth="19425" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Laser" sheetId="5" r:id="rId5"/>
     <sheet name="Emp" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -305,7 +306,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -686,7 +687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -931,16 +932,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="9" width="13.375" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="12" max="12" width="11.375" customWidth="1"/>
+    <col min="13" max="13" width="15.25" customWidth="1"/>
+    <col min="14" max="14" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="14.25" customWidth="1"/>
+    <col min="17" max="17" width="13.375" customWidth="1"/>
+    <col min="18" max="18" width="15.75" customWidth="1"/>
+    <col min="19" max="19" width="12.75" customWidth="1"/>
+    <col min="20" max="20" width="12.375" customWidth="1"/>
+    <col min="21" max="21" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -1013,7 +1033,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1080,7 +1100,7 @@
       </c>
       <c r="B3">
         <f>B2+0.2</f>
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1147,7 +1167,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B10" si="1">B3+0.2</f>
-        <v>2</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1214,7 +1234,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>3.0000000000000004</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1229,7 +1249,7 @@
         <v>5</v>
       </c>
       <c r="G5">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -1281,7 +1301,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
+        <v>3.2000000000000006</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1298,7 +1318,7 @@
       </c>
       <c r="G6">
         <f>G5+0.1</f>
-        <v>1.3</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1350,7 +1370,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>2.6000000000000005</v>
+        <v>3.4000000000000008</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1367,7 +1387,7 @@
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G10" si="3">G6+0.1</f>
-        <v>1.4000000000000001</v>
+        <v>1.8000000000000003</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -1419,7 +1439,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>2.8000000000000007</v>
+        <v>3.600000000000001</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1436,7 +1456,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>1.5000000000000002</v>
+        <v>1.9000000000000004</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -1488,7 +1508,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>3.0000000000000009</v>
+        <v>3.8000000000000012</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1505,7 +1525,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>1.6000000000000003</v>
+        <v>2.0000000000000004</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -1557,7 +1577,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>3.2000000000000011</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1574,7 +1594,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>1.7000000000000004</v>
+        <v>2.1000000000000005</v>
       </c>
       <c r="H10">
         <v>3</v>
@@ -1691,7 +1711,7 @@
       </c>
       <c r="B12">
         <f>B10+0.2</f>
-        <v>3.4000000000000012</v>
+        <v>4.2000000000000011</v>
       </c>
       <c r="C12">
         <f>C2*2</f>
@@ -1710,7 +1730,7 @@
       </c>
       <c r="G12">
         <f>G10+0.1</f>
-        <v>1.8000000000000005</v>
+        <v>2.2000000000000006</v>
       </c>
       <c r="H12">
         <f>H10+1</f>
@@ -1764,7 +1784,7 @@
       </c>
       <c r="B13">
         <f>B12+0.2</f>
-        <v>3.6000000000000014</v>
+        <v>4.4000000000000012</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:D20" si="4">C3*2</f>
@@ -1783,7 +1803,7 @@
       </c>
       <c r="G13">
         <f>G12+0.1</f>
-        <v>1.9000000000000006</v>
+        <v>2.3000000000000007</v>
       </c>
       <c r="H13">
         <v>4</v>
@@ -1836,7 +1856,7 @@
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B20" si="6">B13+0.2</f>
-        <v>3.8000000000000016</v>
+        <v>4.6000000000000014</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
@@ -1855,7 +1875,7 @@
       </c>
       <c r="G14">
         <f t="shared" ref="G14:G20" si="8">G13+0.1</f>
-        <v>2.0000000000000004</v>
+        <v>2.4000000000000008</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -1873,7 +1893,7 @@
         <v>18</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N14">
         <v>30</v>
@@ -1908,7 +1928,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="6"/>
-        <v>4.0000000000000018</v>
+        <v>4.8000000000000016</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
@@ -1927,7 +1947,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="8"/>
-        <v>2.1000000000000005</v>
+        <v>2.5000000000000009</v>
       </c>
       <c r="H15">
         <v>4</v>
@@ -1943,11 +1963,11 @@
         <v>3</v>
       </c>
       <c r="L15">
-        <f>L14+2</f>
-        <v>20</v>
+        <f>L14+5</f>
+        <v>23</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N15">
         <v>30</v>
@@ -1982,7 +2002,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="6"/>
-        <v>4.200000000000002</v>
+        <v>5.0000000000000018</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
@@ -2001,7 +2021,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="8"/>
-        <v>2.2000000000000006</v>
+        <v>2.600000000000001</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -2017,11 +2037,11 @@
         <v>4</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L20" si="11">L15+2</f>
-        <v>22</v>
+        <f t="shared" ref="L16:L20" si="11">L15+5</f>
+        <v>28</v>
       </c>
       <c r="M16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N16">
         <v>30</v>
@@ -2056,7 +2076,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="6"/>
-        <v>4.4000000000000021</v>
+        <v>5.200000000000002</v>
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
@@ -2075,7 +2095,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="8"/>
-        <v>2.3000000000000007</v>
+        <v>2.7000000000000011</v>
       </c>
       <c r="H17">
         <v>4</v>
@@ -2092,10 +2112,10 @@
       </c>
       <c r="L17">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="M17">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N17">
         <v>30</v>
@@ -2130,7 +2150,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="6"/>
-        <v>4.6000000000000023</v>
+        <v>5.4000000000000021</v>
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
@@ -2149,7 +2169,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="8"/>
-        <v>2.4000000000000008</v>
+        <v>2.8000000000000012</v>
       </c>
       <c r="H18">
         <v>4</v>
@@ -2166,10 +2186,10 @@
       </c>
       <c r="L18">
         <f t="shared" si="11"/>
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N18">
         <v>30</v>
@@ -2204,7 +2224,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="6"/>
-        <v>4.8000000000000025</v>
+        <v>5.6000000000000023</v>
       </c>
       <c r="C19">
         <f t="shared" si="4"/>
@@ -2223,7 +2243,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="8"/>
-        <v>2.5000000000000009</v>
+        <v>2.9000000000000012</v>
       </c>
       <c r="H19">
         <v>4</v>
@@ -2240,10 +2260,10 @@
       </c>
       <c r="L19">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N19">
         <v>30</v>
@@ -2278,7 +2298,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="6"/>
-        <v>5.0000000000000027</v>
+        <v>5.8000000000000025</v>
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
@@ -2297,7 +2317,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="8"/>
-        <v>2.600000000000001</v>
+        <v>3.0000000000000013</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -2314,10 +2334,10 @@
       </c>
       <c r="L20">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="M20">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N20">
         <v>30</v>
@@ -2417,11 +2437,11 @@
       </c>
       <c r="B22">
         <f>B20+0.2</f>
-        <v>5.2000000000000028</v>
+        <v>6.0000000000000027</v>
       </c>
       <c r="C22">
-        <f>C12*2</f>
-        <v>4</v>
+        <f>C12*4</f>
+        <v>8</v>
       </c>
       <c r="D22">
         <f>D12*2</f>
@@ -2436,10 +2456,10 @@
       </c>
       <c r="G22">
         <f>G20+0.1</f>
-        <v>2.7000000000000011</v>
+        <v>3.1000000000000014</v>
       </c>
       <c r="H22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I22">
         <v>8</v>
@@ -2451,10 +2471,11 @@
         <v>12</v>
       </c>
       <c r="L22">
-        <v>32</v>
+        <f>L20+7</f>
+        <v>55</v>
       </c>
       <c r="M22">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N22">
         <v>40</v>
@@ -2489,14 +2510,14 @@
       </c>
       <c r="B23">
         <f>B22+0.2</f>
-        <v>5.400000000000003</v>
+        <v>6.2000000000000028</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:D30" si="12">C13*2</f>
-        <v>4</v>
+        <f>C13*4</f>
+        <v>8</v>
       </c>
       <c r="D23">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D23:D30" si="12">D13*2</f>
         <v>4</v>
       </c>
       <c r="E23">
@@ -2507,11 +2528,11 @@
         <v>35</v>
       </c>
       <c r="G23">
-        <f>G22+0.1</f>
-        <v>2.8000000000000012</v>
+        <f>G22+3</f>
+        <v>6.1000000000000014</v>
       </c>
       <c r="H23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I23">
         <v>8</v>
@@ -2524,10 +2545,11 @@
         <v>13</v>
       </c>
       <c r="L23">
-        <v>32</v>
+        <f>L22+7</f>
+        <v>62</v>
       </c>
       <c r="M23">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N23">
         <v>40</v>
@@ -2562,11 +2584,11 @@
       </c>
       <c r="B24">
         <f t="shared" ref="B24:B30" si="14">B23+0.2</f>
-        <v>5.6000000000000032</v>
+        <v>6.400000000000003</v>
       </c>
       <c r="C24">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" ref="C24:C30" si="15">C14*4</f>
+        <v>8</v>
       </c>
       <c r="D24">
         <f t="shared" si="12"/>
@@ -2576,15 +2598,15 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F30" si="15">F23+2</f>
+        <f t="shared" ref="F24:F30" si="16">F23+2</f>
         <v>37</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G30" si="16">G23+0.1</f>
-        <v>2.9000000000000012</v>
+        <f t="shared" ref="G24:G30" si="17">G23+3</f>
+        <v>9.1000000000000014</v>
       </c>
       <c r="H24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>8</v>
@@ -2593,14 +2615,15 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24:K30" si="17">K23+1</f>
+        <f t="shared" ref="K24:K30" si="18">K23+1</f>
         <v>14</v>
       </c>
       <c r="L24">
-        <v>32</v>
+        <f t="shared" ref="L24:L30" si="19">L23+7</f>
+        <v>69</v>
       </c>
       <c r="M24">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N24">
         <v>40</v>
@@ -2612,10 +2635,10 @@
         <v>5</v>
       </c>
       <c r="Q24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S24">
         <v>8</v>
@@ -2624,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="U24">
-        <f t="shared" ref="U24:U30" si="18">U23</f>
+        <f t="shared" ref="U24:U30" si="20">U23</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -2635,11 +2658,11 @@
       </c>
       <c r="B25">
         <f t="shared" si="14"/>
-        <v>5.8000000000000034</v>
+        <v>6.6000000000000032</v>
       </c>
       <c r="C25">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D25">
         <f t="shared" si="12"/>
@@ -2649,15 +2672,15 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>39</v>
       </c>
       <c r="G25">
-        <f t="shared" si="16"/>
-        <v>3.0000000000000013</v>
+        <f t="shared" si="17"/>
+        <v>12.100000000000001</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I25">
         <v>8</v>
@@ -2666,14 +2689,15 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="L25">
-        <v>32</v>
+        <f t="shared" si="19"/>
+        <v>76</v>
       </c>
       <c r="M25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N25">
         <v>40</v>
@@ -2686,11 +2710,11 @@
         <v>8</v>
       </c>
       <c r="Q25">
-        <f>Q24+0.2</f>
-        <v>6.2</v>
+        <f>Q24+0.5</f>
+        <v>10.5</v>
       </c>
       <c r="R25">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S25">
         <v>8</v>
@@ -2699,7 +2723,7 @@
         <v>3</v>
       </c>
       <c r="U25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -2710,11 +2734,11 @@
       </c>
       <c r="B26">
         <f t="shared" si="14"/>
-        <v>6.0000000000000036</v>
+        <v>6.8000000000000034</v>
       </c>
       <c r="C26">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D26">
         <f t="shared" si="12"/>
@@ -2724,15 +2748,15 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>41</v>
       </c>
       <c r="G26">
-        <f t="shared" si="16"/>
-        <v>3.1000000000000014</v>
+        <f t="shared" si="17"/>
+        <v>15.100000000000001</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I26">
         <v>8</v>
@@ -2741,14 +2765,15 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="L26">
-        <v>36</v>
+        <f t="shared" si="19"/>
+        <v>83</v>
       </c>
       <c r="M26">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N26">
         <v>40</v>
@@ -2757,15 +2782,15 @@
         <v>5</v>
       </c>
       <c r="P26">
-        <f t="shared" ref="P26:P30" si="19">P25+3</f>
+        <f t="shared" ref="P26:P30" si="21">P25+3</f>
         <v>11</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26:Q30" si="20">Q25+0.2</f>
-        <v>6.4</v>
+        <f t="shared" ref="Q26" si="22">Q25+0.5</f>
+        <v>11</v>
       </c>
       <c r="R26">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S26">
         <v>8</v>
@@ -2774,7 +2799,7 @@
         <v>3</v>
       </c>
       <c r="U26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -2785,11 +2810,11 @@
       </c>
       <c r="B27">
         <f t="shared" si="14"/>
-        <v>6.2000000000000037</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="C27">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D27">
         <f t="shared" si="12"/>
@@ -2799,15 +2824,15 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43</v>
       </c>
       <c r="G27">
-        <f t="shared" si="16"/>
-        <v>3.2000000000000015</v>
+        <f t="shared" si="17"/>
+        <v>18.100000000000001</v>
       </c>
       <c r="H27">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I27">
         <v>8</v>
@@ -2816,14 +2841,15 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="L27">
-        <v>36</v>
+        <f t="shared" si="19"/>
+        <v>90</v>
       </c>
       <c r="M27">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N27">
         <v>40</v>
@@ -2832,15 +2858,14 @@
         <v>5</v>
       </c>
       <c r="P27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>14</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="20"/>
-        <v>6.6000000000000005</v>
+        <v>14</v>
       </c>
       <c r="R27">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S27">
         <v>8</v>
@@ -2849,7 +2874,7 @@
         <v>3</v>
       </c>
       <c r="U27">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -2860,11 +2885,11 @@
       </c>
       <c r="B28">
         <f t="shared" si="14"/>
-        <v>6.4000000000000039</v>
+        <v>7.2000000000000037</v>
       </c>
       <c r="C28">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D28">
         <f t="shared" si="12"/>
@@ -2874,15 +2899,15 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="G28">
-        <f t="shared" si="16"/>
-        <v>3.3000000000000016</v>
+        <f t="shared" si="17"/>
+        <v>21.1</v>
       </c>
       <c r="H28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I28">
         <v>8</v>
@@ -2891,14 +2916,15 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="L28">
-        <v>36</v>
+        <f t="shared" si="19"/>
+        <v>97</v>
       </c>
       <c r="M28">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N28">
         <v>40</v>
@@ -2907,15 +2933,15 @@
         <v>5</v>
       </c>
       <c r="P28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="20"/>
-        <v>6.8000000000000007</v>
+        <f>Q27+2</f>
+        <v>16</v>
       </c>
       <c r="R28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S28">
         <v>8</v>
@@ -2924,7 +2950,7 @@
         <v>3</v>
       </c>
       <c r="U28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -2935,11 +2961,11 @@
       </c>
       <c r="B29">
         <f t="shared" si="14"/>
-        <v>6.6000000000000041</v>
+        <v>7.4000000000000039</v>
       </c>
       <c r="C29">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D29">
         <f t="shared" si="12"/>
@@ -2949,15 +2975,15 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>47</v>
       </c>
       <c r="G29">
-        <f t="shared" si="16"/>
-        <v>3.4000000000000017</v>
+        <f t="shared" si="17"/>
+        <v>24.1</v>
       </c>
       <c r="H29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I29">
         <v>8</v>
@@ -2966,14 +2992,15 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>19</v>
       </c>
       <c r="L29">
-        <v>36</v>
+        <f t="shared" si="19"/>
+        <v>104</v>
       </c>
       <c r="M29">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N29">
         <v>40</v>
@@ -2982,15 +3009,15 @@
         <v>5</v>
       </c>
       <c r="P29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="20"/>
-        <v>7.0000000000000009</v>
+        <f t="shared" ref="Q29:Q30" si="23">Q28+2</f>
+        <v>18</v>
       </c>
       <c r="R29">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S29">
         <v>8</v>
@@ -2999,7 +3026,7 @@
         <v>3</v>
       </c>
       <c r="U29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -3010,11 +3037,11 @@
       </c>
       <c r="B30">
         <f t="shared" si="14"/>
-        <v>6.8000000000000043</v>
+        <v>7.6000000000000041</v>
       </c>
       <c r="C30">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="D30">
         <f t="shared" si="12"/>
@@ -3024,15 +3051,15 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>49</v>
       </c>
       <c r="G30">
-        <f t="shared" si="16"/>
-        <v>3.5000000000000018</v>
+        <f t="shared" si="17"/>
+        <v>27.1</v>
       </c>
       <c r="H30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I30">
         <v>8</v>
@@ -3041,14 +3068,15 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="L30">
-        <v>36</v>
+        <f t="shared" si="19"/>
+        <v>111</v>
       </c>
       <c r="M30">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N30">
         <v>40</v>
@@ -3057,15 +3085,15 @@
         <v>5</v>
       </c>
       <c r="P30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>23</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="20"/>
-        <v>7.2000000000000011</v>
+        <f t="shared" si="23"/>
+        <v>20</v>
       </c>
       <c r="R30">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S30">
         <v>8</v>
@@ -3074,7 +3102,7 @@
         <v>3</v>
       </c>
       <c r="U30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -3150,11 +3178,11 @@
       </c>
       <c r="B32">
         <f>B30+0.2</f>
-        <v>7.0000000000000044</v>
+        <v>7.8000000000000043</v>
       </c>
       <c r="C32">
         <f>C22*2</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D32">
         <f>D22*2</f>
@@ -3168,11 +3196,11 @@
         <v>51</v>
       </c>
       <c r="G32">
-        <f>G30+0.1</f>
-        <v>3.6000000000000019</v>
+        <f>G30+3</f>
+        <v>30.1</v>
       </c>
       <c r="H32">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I32">
         <v>16</v>
@@ -3184,10 +3212,11 @@
         <v>24</v>
       </c>
       <c r="L32">
-        <v>40</v>
+        <f>L30+8</f>
+        <v>119</v>
       </c>
       <c r="M32">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N32">
         <v>50</v>
@@ -3200,11 +3229,11 @@
         <v>26</v>
       </c>
       <c r="Q32">
-        <f>Q30+0.2</f>
-        <v>7.4000000000000012</v>
+        <f>Q30+8</f>
+        <v>28</v>
       </c>
       <c r="R32">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S32">
         <v>16</v>
@@ -3224,14 +3253,14 @@
       </c>
       <c r="B33">
         <f>B32+0.2</f>
-        <v>7.2000000000000046</v>
+        <v>8.0000000000000036</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:D42" si="21">C23*2</f>
-        <v>8</v>
+        <f t="shared" ref="C33:D40" si="24">C23*2</f>
+        <v>16</v>
       </c>
       <c r="D33">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="E33">
@@ -3242,11 +3271,11 @@
         <v>53</v>
       </c>
       <c r="G33">
-        <f>G32+0.1</f>
-        <v>3.700000000000002</v>
+        <f>G32+3</f>
+        <v>33.1</v>
       </c>
       <c r="H33">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I33">
         <v>16</v>
@@ -3259,10 +3288,11 @@
         <v>25</v>
       </c>
       <c r="L33">
-        <v>40</v>
+        <f>L32+8</f>
+        <v>127</v>
       </c>
       <c r="M33">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N33">
         <v>50</v>
@@ -3275,11 +3305,11 @@
         <v>29</v>
       </c>
       <c r="Q33">
-        <f>Q32+0.2</f>
-        <v>7.6000000000000014</v>
+        <f>Q32+8</f>
+        <v>36</v>
       </c>
       <c r="R33">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S33">
         <v>16</v>
@@ -3294,34 +3324,34 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" ref="A34:A42" si="22">A33+2</f>
+        <f t="shared" ref="A34:A40" si="25">A33+2</f>
         <v>68</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:B42" si="23">B33+0.2</f>
-        <v>7.4000000000000048</v>
+        <f t="shared" ref="B34:B40" si="26">B33+0.2</f>
+        <v>8.2000000000000028</v>
       </c>
       <c r="C34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F42" si="24">F33+2</f>
+        <f t="shared" ref="F34:F40" si="27">F33+2</f>
         <v>55</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G42" si="25">G33+0.1</f>
-        <v>3.800000000000002</v>
+        <f t="shared" ref="G34:G41" si="28">G33+3</f>
+        <v>36.1</v>
       </c>
       <c r="H34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I34">
         <v>16</v>
@@ -3330,14 +3360,15 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34:K42" si="26">K33+1</f>
+        <f t="shared" ref="K34:K40" si="29">K33+1</f>
         <v>26</v>
       </c>
       <c r="L34">
-        <v>40</v>
+        <f t="shared" ref="L34:L40" si="30">L33+8</f>
+        <v>135</v>
       </c>
       <c r="M34">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N34">
         <v>50</v>
@@ -3346,15 +3377,15 @@
         <v>5</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34:P42" si="27">P33+3</f>
+        <f t="shared" ref="P34:P40" si="31">P33+3</f>
         <v>32</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34:Q42" si="28">Q33+0.2</f>
-        <v>7.8000000000000016</v>
+        <f t="shared" ref="Q34:Q37" si="32">Q33+8</f>
+        <v>44</v>
       </c>
       <c r="R34">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S34">
         <v>16</v>
@@ -3363,40 +3394,40 @@
         <v>3</v>
       </c>
       <c r="U34">
-        <f t="shared" ref="U34:U42" si="29">U33</f>
+        <f t="shared" ref="U34:U40" si="33">U33</f>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>70</v>
       </c>
       <c r="B35">
-        <f t="shared" si="23"/>
-        <v>7.600000000000005</v>
+        <f t="shared" si="26"/>
+        <v>8.4000000000000021</v>
       </c>
       <c r="C35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>57</v>
       </c>
       <c r="G35">
-        <f t="shared" si="25"/>
-        <v>3.9000000000000021</v>
+        <f t="shared" si="28"/>
+        <v>39.1</v>
       </c>
       <c r="H35">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I35">
         <v>16</v>
@@ -3405,14 +3436,15 @@
         <v>1</v>
       </c>
       <c r="K35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>27</v>
       </c>
       <c r="L35">
-        <v>40</v>
+        <f t="shared" si="30"/>
+        <v>143</v>
       </c>
       <c r="M35">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N35">
         <v>50</v>
@@ -3421,15 +3453,15 @@
         <v>5</v>
       </c>
       <c r="P35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>35</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000018</v>
+        <f t="shared" si="32"/>
+        <v>52</v>
       </c>
       <c r="R35">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S35">
         <v>16</v>
@@ -3438,40 +3470,40 @@
         <v>3</v>
       </c>
       <c r="U35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>72</v>
       </c>
       <c r="B36">
-        <f t="shared" si="23"/>
-        <v>7.8000000000000052</v>
+        <f t="shared" si="26"/>
+        <v>8.6000000000000014</v>
       </c>
       <c r="C36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>59</v>
       </c>
       <c r="G36">
-        <f t="shared" si="25"/>
-        <v>4.0000000000000018</v>
+        <f t="shared" si="28"/>
+        <v>42.1</v>
       </c>
       <c r="H36">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I36">
         <v>16</v>
@@ -3480,14 +3512,15 @@
         <v>1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>28</v>
       </c>
       <c r="L36">
-        <v>40</v>
+        <f>L35+15</f>
+        <v>158</v>
       </c>
       <c r="M36">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N36">
         <v>50</v>
@@ -3496,15 +3529,15 @@
         <v>5</v>
       </c>
       <c r="P36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>38</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="28"/>
-        <v>8.2000000000000011</v>
+        <f t="shared" si="32"/>
+        <v>60</v>
       </c>
       <c r="R36">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S36">
         <v>16</v>
@@ -3513,40 +3546,40 @@
         <v>3</v>
       </c>
       <c r="U36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>74</v>
       </c>
       <c r="B37">
-        <f t="shared" si="23"/>
-        <v>8.0000000000000053</v>
+        <f t="shared" si="26"/>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C37">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>61</v>
       </c>
       <c r="G37">
-        <f t="shared" si="25"/>
-        <v>4.1000000000000014</v>
+        <f t="shared" si="28"/>
+        <v>45.1</v>
       </c>
       <c r="H37">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I37">
         <v>16</v>
@@ -3555,14 +3588,15 @@
         <v>1</v>
       </c>
       <c r="K37">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>29</v>
       </c>
       <c r="L37">
-        <v>44</v>
+        <f t="shared" ref="L37:L40" si="34">L36+15</f>
+        <v>173</v>
       </c>
       <c r="M37">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N37">
         <v>50</v>
@@ -3571,15 +3605,15 @@
         <v>5</v>
       </c>
       <c r="P37">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>41</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="28"/>
-        <v>8.4</v>
+        <f t="shared" si="32"/>
+        <v>68</v>
       </c>
       <c r="R37">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S37">
         <v>16</v>
@@ -3588,40 +3622,40 @@
         <v>3</v>
       </c>
       <c r="U37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>76</v>
       </c>
       <c r="B38">
-        <f t="shared" si="23"/>
-        <v>8.2000000000000046</v>
+        <f t="shared" si="26"/>
+        <v>9</v>
       </c>
       <c r="C38">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>63</v>
       </c>
       <c r="G38">
-        <f t="shared" si="25"/>
-        <v>4.2000000000000011</v>
+        <f t="shared" si="28"/>
+        <v>48.1</v>
       </c>
       <c r="H38">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I38">
         <v>16</v>
@@ -3630,14 +3664,15 @@
         <v>1</v>
       </c>
       <c r="K38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>30</v>
       </c>
       <c r="L38">
-        <v>44</v>
+        <f t="shared" si="34"/>
+        <v>188</v>
       </c>
       <c r="M38">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N38">
         <v>50</v>
@@ -3646,15 +3681,15 @@
         <v>5</v>
       </c>
       <c r="P38">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>44</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="28"/>
-        <v>8.6</v>
+        <f>Q37+12</f>
+        <v>80</v>
       </c>
       <c r="R38">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S38">
         <v>16</v>
@@ -3663,40 +3698,40 @@
         <v>3</v>
       </c>
       <c r="U38">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>78</v>
       </c>
       <c r="B39">
-        <f t="shared" si="23"/>
-        <v>8.4000000000000039</v>
+        <f t="shared" si="26"/>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C39">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>65</v>
       </c>
       <c r="G39">
-        <f t="shared" si="25"/>
-        <v>4.3000000000000007</v>
+        <f t="shared" si="28"/>
+        <v>51.1</v>
       </c>
       <c r="H39">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I39">
         <v>16</v>
@@ -3705,14 +3740,15 @@
         <v>1</v>
       </c>
       <c r="K39">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>31</v>
       </c>
       <c r="L39">
-        <v>44</v>
+        <f t="shared" si="34"/>
+        <v>203</v>
       </c>
       <c r="M39">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N39">
         <v>50</v>
@@ -3721,15 +3757,15 @@
         <v>5</v>
       </c>
       <c r="P39">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>47</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="28"/>
-        <v>8.7999999999999989</v>
+        <f t="shared" ref="Q39:Q40" si="35">Q38+12</f>
+        <v>92</v>
       </c>
       <c r="R39">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S39">
         <v>16</v>
@@ -3738,40 +3774,40 @@
         <v>3</v>
       </c>
       <c r="U39">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>80</v>
       </c>
       <c r="B40">
-        <f t="shared" si="23"/>
-        <v>8.6000000000000032</v>
+        <f t="shared" si="26"/>
+        <v>9.3999999999999986</v>
       </c>
       <c r="C40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="D40">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>67</v>
       </c>
       <c r="G40">
-        <f t="shared" si="25"/>
-        <v>4.4000000000000004</v>
+        <f t="shared" si="28"/>
+        <v>54.1</v>
       </c>
       <c r="H40">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I40">
         <v>16</v>
@@ -3780,14 +3816,15 @@
         <v>1</v>
       </c>
       <c r="K40">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
       <c r="L40">
-        <v>44</v>
+        <f t="shared" si="34"/>
+        <v>218</v>
       </c>
       <c r="M40">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N40">
         <v>50</v>
@@ -3796,15 +3833,15 @@
         <v>5</v>
       </c>
       <c r="P40">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>50</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="28"/>
-        <v>8.9999999999999982</v>
+        <f t="shared" si="35"/>
+        <v>104</v>
       </c>
       <c r="R40">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="S40">
         <v>16</v>
@@ -3813,7 +3850,7 @@
         <v>3</v>
       </c>
       <c r="U40">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.40000000000000008</v>
       </c>
     </row>
@@ -3837,7 +3874,8 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>57.1</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3954,11 +3992,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3994,10 +4032,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>5000</v>
@@ -4016,12 +4054,12 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f>D2+200</f>
-        <v>700</v>
+        <f>D2+100</f>
+        <v>200</v>
       </c>
       <c r="E3">
-        <f>E2+200</f>
-        <v>700</v>
+        <f>E2+100</f>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -4040,12 +4078,12 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="2">D3+200</f>
-        <v>900</v>
+        <f t="shared" ref="D4:D20" si="2">D3+100</f>
+        <v>300</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="3">E3+200</f>
-        <v>900</v>
+        <f t="shared" ref="E4:E20" si="3">E3+100</f>
+        <v>300</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -4065,11 +4103,11 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -4089,11 +4127,11 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -4113,11 +4151,11 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F7">
         <v>-1</v>
@@ -4137,11 +4175,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -4161,11 +4199,11 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -4185,11 +4223,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -4209,11 +4247,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -4233,11 +4271,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -4257,11 +4295,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -4281,11 +4319,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -4305,11 +4343,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="F15">
         <v>-1</v>
@@ -4329,11 +4367,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="F16">
         <v>-1</v>
@@ -4353,11 +4391,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="F17">
         <v>-1</v>
@@ -4377,11 +4415,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="F18">
         <v>-1</v>
@@ -4401,11 +4439,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="F19">
         <v>-1</v>
@@ -4425,11 +4463,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="F20">
         <v>-1</v>
@@ -4464,11 +4502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4504,10 +4542,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>5000</v>
@@ -4526,12 +4564,12 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <f>D2+200</f>
-        <v>700</v>
+        <f>D2+100</f>
+        <v>200</v>
       </c>
       <c r="E3">
-        <f>E2+200</f>
-        <v>700</v>
+        <f>E2+100</f>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -4550,12 +4588,12 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="2">D3+200</f>
-        <v>900</v>
+        <f t="shared" ref="D4:D20" si="2">D3+100</f>
+        <v>300</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="3">E3+200</f>
-        <v>900</v>
+        <f t="shared" ref="E4:E20" si="3">E3+100</f>
+        <v>300</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -4575,11 +4613,11 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -4599,11 +4637,11 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -4623,11 +4661,11 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F7">
         <v>-1</v>
@@ -4647,11 +4685,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -4671,11 +4709,11 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -4695,11 +4733,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -4719,11 +4757,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -4743,11 +4781,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -4767,11 +4805,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -4791,11 +4829,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -4815,11 +4853,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="F15">
         <v>-1</v>
@@ -4839,11 +4877,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="F16">
         <v>-1</v>
@@ -4863,11 +4901,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="F17">
         <v>-1</v>
@@ -4887,11 +4925,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="F18">
         <v>-1</v>
@@ -4911,11 +4949,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="F19">
         <v>-1</v>
@@ -4935,11 +4973,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="F20">
         <v>-1</v>
@@ -4965,11 +5003,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E3" sqref="E3:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5005,10 +5043,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>5000</v>
@@ -5027,12 +5065,12 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>D2+200</f>
-        <v>700</v>
+        <f>D2+100</f>
+        <v>200</v>
       </c>
       <c r="E3">
-        <f>E2+200</f>
-        <v>700</v>
+        <f>E2+100</f>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -5051,12 +5089,12 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="2">D3+200</f>
-        <v>900</v>
+        <f t="shared" ref="D4:D20" si="2">D3+100</f>
+        <v>300</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="3">E3+200</f>
-        <v>900</v>
+        <f t="shared" ref="E4:E20" si="3">E3+100</f>
+        <v>300</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -5076,11 +5114,11 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -5100,11 +5138,11 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -5124,11 +5162,11 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F7">
         <v>-1</v>
@@ -5148,11 +5186,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -5172,11 +5210,11 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -5196,11 +5234,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -5220,11 +5258,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -5244,11 +5282,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -5268,11 +5306,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -5292,11 +5330,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -5316,11 +5354,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="F15">
         <v>-1</v>
@@ -5340,11 +5378,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="F16">
         <v>-1</v>
@@ -5364,11 +5402,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="F17">
         <v>-1</v>
@@ -5388,11 +5426,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="F18">
         <v>-1</v>
@@ -5412,11 +5450,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="F19">
         <v>-1</v>
@@ -5436,11 +5474,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="F20">
         <v>-1</v>
@@ -5466,11 +5504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E3" sqref="E3:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5506,10 +5544,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>5000</v>
@@ -5528,12 +5566,12 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>D2+200</f>
-        <v>700</v>
+        <f>D2+100</f>
+        <v>200</v>
       </c>
       <c r="E3">
-        <f>E2+200</f>
-        <v>700</v>
+        <f>E2+100</f>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -5552,12 +5590,12 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D20" si="2">D3+200</f>
-        <v>900</v>
+        <f t="shared" ref="D4:D20" si="2">D3+100</f>
+        <v>300</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="3">E3+200</f>
-        <v>900</v>
+        <f t="shared" ref="E4:E20" si="3">E3+100</f>
+        <v>300</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -5577,11 +5615,11 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -5601,11 +5639,11 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -5625,11 +5663,11 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F7">
         <v>-1</v>
@@ -5649,11 +5687,11 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -5673,11 +5711,11 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>1900</v>
+        <v>800</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -5697,11 +5735,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -5721,11 +5759,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -5745,11 +5783,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -5769,11 +5807,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -5793,11 +5831,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>2900</v>
+        <v>1300</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -5817,11 +5855,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>3100</v>
+        <v>1400</v>
       </c>
       <c r="F15">
         <v>-1</v>
@@ -5841,11 +5879,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>3300</v>
+        <v>1500</v>
       </c>
       <c r="F16">
         <v>-1</v>
@@ -5865,11 +5903,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="F17">
         <v>-1</v>
@@ -5889,11 +5927,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="F18">
         <v>-1</v>
@@ -5913,11 +5951,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="F19">
         <v>-1</v>
@@ -5937,11 +5975,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>1900</v>
       </c>
       <c r="F20">
         <v>-1</v>

</xml_diff>

<commit_message>
EMP Balancing Finsih, Achievement Jem
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/DataBase.xlsx
+++ b/Assets/8. Execl/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A221C55-E38F-4E7D-88A4-F1F099A4AE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FA885B-6521-46C8-B1C9-3039D04B5C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>achieveName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -248,10 +248,6 @@
     <t>expertSkillUpgradeJem</t>
   </si>
   <si>
-    <t>3000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1000,2000,3000,4000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -259,34 +255,10 @@
     <t>500,1000,1500,2000</t>
   </si>
   <si>
-    <t>500,1000,1500,2000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>100,200,300,400</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>100,300,500,700</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5,10,15,20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4,8,12,16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3,6,9,12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2,5,8,11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>All in game status level 30</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -300,6 +272,38 @@
   </si>
   <si>
     <t>Survive 30 Sec in Bouns Wave</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,200,400,800</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,100,300,500</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,100,200,400</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,4,7,10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,5,9,13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,6,11,16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,5,7</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -690,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -731,10 +735,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -748,10 +752,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -765,10 +769,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -782,10 +786,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -799,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -816,10 +820,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -833,10 +837,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -850,10 +854,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -861,7 +865,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -870,7 +874,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -878,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -887,7 +891,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,7 +899,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -904,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -912,7 +916,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -921,7 +925,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -935,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -1157,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -1224,7 +1228,7 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -1291,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1360,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1429,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -1498,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1567,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -1636,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1773,8 +1777,8 @@
         <v>0</v>
       </c>
       <c r="U12">
-        <f>U10-0.2</f>
-        <v>0.8</v>
+        <f>U10-0.4</f>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1846,7 +1850,7 @@
       </c>
       <c r="U13">
         <f>U12</f>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1918,7 +1922,7 @@
       </c>
       <c r="U14">
         <f t="shared" ref="U14:U20" si="9">U13</f>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -1992,7 +1996,7 @@
       </c>
       <c r="U15">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -2066,7 +2070,7 @@
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -2140,7 +2144,7 @@
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -2214,7 +2218,7 @@
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -2288,7 +2292,7 @@
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -2362,7 +2366,7 @@
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -2500,7 +2504,7 @@
       </c>
       <c r="U22">
         <f>U12-0.2</f>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -2574,7 +2578,7 @@
       </c>
       <c r="U23">
         <f>U22</f>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -2648,7 +2652,7 @@
       </c>
       <c r="U24">
         <f t="shared" ref="U24:U30" si="19">U23</f>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -2724,7 +2728,7 @@
       </c>
       <c r="U25">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -2800,7 +2804,7 @@
       </c>
       <c r="U26">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -2875,7 +2879,7 @@
       </c>
       <c r="U27">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -2951,7 +2955,7 @@
       </c>
       <c r="U28">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -3027,7 +3031,7 @@
       </c>
       <c r="U29">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -3103,7 +3107,7 @@
       </c>
       <c r="U30">
         <f t="shared" si="19"/>
-        <v>0.60000000000000009</v>
+        <v>0.59999999999999987</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
@@ -3243,7 +3247,7 @@
       </c>
       <c r="U32">
         <f>U22-0.2</f>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -3319,7 +3323,7 @@
       </c>
       <c r="U33">
         <f>U32</f>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3395,7 +3399,7 @@
       </c>
       <c r="U34">
         <f t="shared" ref="U34:U40" si="34">U33</f>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -3471,7 +3475,7 @@
       </c>
       <c r="U35">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -3547,7 +3551,7 @@
       </c>
       <c r="U36">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -3623,7 +3627,7 @@
       </c>
       <c r="U37">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -3699,7 +3703,7 @@
       </c>
       <c r="U38">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -3775,7 +3779,7 @@
       </c>
       <c r="U39">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -3851,7 +3855,7 @@
       </c>
       <c r="U40">
         <f t="shared" si="34"/>
-        <v>0.40000000000000008</v>
+        <v>0.39999999999999986</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
@@ -3924,64 +3928,64 @@
         <v>1</v>
       </c>
       <c r="B42">
-        <v>8.6</v>
+        <v>200</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D42">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42">
-        <v>4.4000000000000004</v>
+        <v>150</v>
       </c>
       <c r="H42">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="I42">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42">
-        <v>44</v>
+        <v>400</v>
       </c>
       <c r="M42">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="N42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O42">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P42">
         <v>1</v>
       </c>
       <c r="Q42">
-        <v>9</v>
+        <v>300</v>
       </c>
       <c r="R42">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="S42">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="T42">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="U42">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -4504,7 +4508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -4580,7 +4584,7 @@
         <v>0.2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B21" si="1">B3-0.015</f>
+        <f t="shared" ref="B4:B19" si="1">B3-0.015</f>
         <v>0.77</v>
       </c>
       <c r="C4">
@@ -5507,7 +5511,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5534,7 +5538,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
       <c r="B2">
         <v>0.25</v>
@@ -5549,16 +5553,16 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <v>5000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>A2+0.025</f>
-        <v>0.17499999999999999</v>
+        <f>A2+0.05</f>
+        <v>0.75</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B21" si="0">B2+0.005</f>
+        <f t="shared" ref="B3:B11" si="0">B2+0.005</f>
         <v>0.255</v>
       </c>
       <c r="C3">
@@ -5578,8 +5582,8 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="1">A3+0.025</f>
-        <v>0.19999999999999998</v>
+        <f t="shared" ref="A4:A6" si="1">A3+0.05</f>
+        <v>0.8</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -5603,7 +5607,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>0.22499999999999998</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -5627,7 +5631,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>0.24999999999999997</v>
+        <v>0.90000000000000013</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -5650,8 +5654,8 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="1"/>
-        <v>0.27499999999999997</v>
+        <f t="shared" ref="A7:A10" si="4">A6+0.07</f>
+        <v>0.9700000000000002</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -5674,8 +5678,8 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>1.0400000000000003</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -5698,8 +5702,8 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="1"/>
-        <v>0.32500000000000001</v>
+        <f t="shared" si="4"/>
+        <v>1.1100000000000003</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -5722,8 +5726,8 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
+        <f t="shared" si="4"/>
+        <v>1.1800000000000004</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -5746,8 +5750,8 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="1"/>
-        <v>0.37500000000000006</v>
+        <f>A10+0.07</f>
+        <v>1.2500000000000004</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -5770,12 +5774,12 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="1"/>
-        <v>0.40000000000000008</v>
+        <f>A11+0.1</f>
+        <v>1.3500000000000005</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" ref="B12:B21" si="5">B11+0.01</f>
+        <v>0.30500000000000005</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -5794,12 +5798,12 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="1"/>
-        <v>0.4250000000000001</v>
+        <f>A12+0.2</f>
+        <v>1.5500000000000005</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>0.30500000000000005</v>
+        <f t="shared" si="5"/>
+        <v>0.31500000000000006</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -5818,12 +5822,12 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="1"/>
-        <v>0.45000000000000012</v>
+        <f t="shared" ref="A14:A15" si="6">A13+0.2</f>
+        <v>1.7500000000000004</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>0.31000000000000005</v>
+        <f t="shared" si="5"/>
+        <v>0.32500000000000007</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -5842,12 +5846,12 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="1"/>
-        <v>0.47500000000000014</v>
+        <f t="shared" si="6"/>
+        <v>1.9500000000000004</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0.31500000000000006</v>
+        <f t="shared" si="5"/>
+        <v>0.33500000000000008</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -5866,12 +5870,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="1"/>
-        <v>0.50000000000000011</v>
+        <f>A15+0.3</f>
+        <v>2.2500000000000004</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0.32000000000000006</v>
+        <f t="shared" si="5"/>
+        <v>0.34500000000000008</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -5890,12 +5894,12 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="1"/>
-        <v>0.52500000000000013</v>
+        <f>A16+0.3</f>
+        <v>2.5500000000000003</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>0.32500000000000007</v>
+        <f t="shared" si="5"/>
+        <v>0.35500000000000009</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -5914,12 +5918,12 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000016</v>
+        <f>A17+0.3</f>
+        <v>2.85</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>0.33000000000000007</v>
+        <f t="shared" si="5"/>
+        <v>0.3650000000000001</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -5938,12 +5942,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="1"/>
-        <v>0.57500000000000018</v>
+        <f>A18+0.5</f>
+        <v>3.35</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>0.33500000000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.37500000000000011</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -5962,12 +5966,12 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="1"/>
-        <v>0.6000000000000002</v>
+        <f t="shared" ref="A20:A21" si="7">A19+0.5</f>
+        <v>3.85</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0.34000000000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.38500000000000012</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -5986,12 +5990,12 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="1"/>
-        <v>0.62500000000000022</v>
+        <f t="shared" si="7"/>
+        <v>4.3499999999999996</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>0.34500000000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.39500000000000013</v>
       </c>
       <c r="C21">
         <v>-1</v>

</xml_diff>